<commit_message>
Print COA _v5 (belum optimisasi)
</commit_message>
<xml_diff>
--- a/TEMPLATE_COA_BUSBAR.xlsx
+++ b/TEMPLATE_COA_BUSBAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrrx\Documents\My Web Sites\H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831617AA-DAD6-4A93-940D-F123D27B6172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC06AD17-4260-403E-8DB8-19E9BA24B771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="A" sheetId="27" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">A!$B$1:$K$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">A!$B$1:$K$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3037,48 +3037,6 @@
     <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3096,15 +3054,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="21" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="24" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3122,6 +3071,57 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2346">
@@ -5487,157 +5487,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2643187</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>361715</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3092363</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1329592</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95BD6E30-1539-4C07-9E5C-C4732E0F4E3F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="29341762" y="23774165"/>
-          <a:ext cx="3621001" cy="4263527"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="2500">
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>Approved</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="2500" baseline="0">
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t> By</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="2500" baseline="0">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="2500" baseline="0">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="2500" baseline="0">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="2500" baseline="0">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="2500" baseline="0">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="2500" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Khilmi Muzakki</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="2500" u="sng">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="2500">
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>(Quality Assurance)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="2500" baseline="0">
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -44838,529 +44687,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>129268</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>692262</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>546136</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1166811</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1019" name="TextBox 1018">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5A0BC83-F0EA-42DC-8113-FAC5E4EB900B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="710293" y="24104712"/>
-          <a:ext cx="7427268" cy="3770199"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>Jl.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t> Manukan Kulon No. 128-130</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>Tandes - Surabaya 60185</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>TEL</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>E-mail</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>Website</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-ID" sz="2500" b="1">
-            <a:solidFill>
-              <a:srgbClr val="EB6C15"/>
-            </a:solidFill>
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1797500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>1483481</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542456</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1463711</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1020" name="TextBox 1019">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D4617A-EACD-47AD-BBE0-0EDA0C8312DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2378525" y="24895931"/>
-          <a:ext cx="8965281" cy="3275880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>:+62 31 - 7491694</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>: marketing@indowire.co.id</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ID" sz="2500" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="EB6C15"/>
-              </a:solidFill>
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>: www.indowire.co.id</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-ID" sz="2500" b="1">
-            <a:solidFill>
-              <a:srgbClr val="EB6C15"/>
-            </a:solidFill>
-            <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>1508125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2730954</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>1317625</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="1209" name="Group 1208">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76457532-4EE2-423B-918B-1EBCA3EE92EB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="584200" y="22869525"/>
-          <a:ext cx="9944554" cy="2984500"/>
-          <a:chOff x="0" y="17380960"/>
-          <a:chExt cx="7453312" cy="2186999"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="1210" name="TextBox 1209">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24DDCDC1-DCC4-5A13-554E-07B1EF42AEFB}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1692416" y="18836332"/>
-            <a:ext cx="3429958" cy="731627"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-ID" sz="1200" b="1">
-                <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>5141/SJ-IND.8/TKDN/6/2023</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-ID" sz="1200" b="1">
-                <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>94.32</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-ID" sz="1200" b="1" baseline="0">
-                <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t> %</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-ID" sz="1200" b="1">
-              <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="1211" name="Group 1210">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1233A0A-F356-A8D2-2C42-C9E2F0FF5A3C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="0" y="17403867"/>
-            <a:ext cx="2437074" cy="2015593"/>
-            <a:chOff x="-753167" y="-95000"/>
-            <a:chExt cx="2228149" cy="1210033"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="1214" name="Picture 1213" descr="A black square with white letters&#10;&#10;Description automatically generated">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF6EEFC6-4646-FFD9-FF42-7E4169E3EA13}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill rotWithShape="1">
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-              <a:extLst>
-                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-                </a:ext>
-              </a:extLst>
-            </a:blip>
-            <a:srcRect l="28184" t="15435" r="25564" b="12706"/>
-            <a:stretch/>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="-361418" y="-95000"/>
-              <a:ext cx="1341256" cy="862322"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1215" name="Text Box 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28638A2B-A1EB-4BAE-A631-8E3095DD68C2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="-753167" y="803293"/>
-              <a:ext cx="2228149" cy="311740"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="6350">
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
-              <a:prstTxWarp prst="textNoShape">
-                <a:avLst/>
-              </a:prstTxWarp>
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr">
-                <a:lnSpc>
-                  <a:spcPct val="107000"/>
-                </a:lnSpc>
-                <a:spcAft>
-                  <a:spcPts val="800"/>
-                </a:spcAft>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1200" b="1" kern="100">
-                  <a:effectLst/>
-                  <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-                  <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>8760:2019</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-ID" sz="1200" kern="100">
-                <a:effectLst/>
-                <a:latin typeface="Montserrat" panose="00000500000000000000" pitchFamily="2" charset="0"/>
-                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="1212" name="Picture 1211">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53296A26-CEE4-DEF1-855F-4834DBC9B3B8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2570905" y="17380960"/>
-            <a:ext cx="1558582" cy="1488792"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="1213" name="Picture 1212">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC7B722E-27CD-5E0A-DB5A-563104FEEC2F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-          <a:srcRect t="2612" b="1"/>
-          <a:stretch/>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4357688" y="17383123"/>
-            <a:ext cx="3095624" cy="1533451"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -45790,8 +45116,8 @@
   </sheetPr>
   <dimension ref="B1:Q38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B18" zoomScale="30" zoomScaleNormal="91" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B2" zoomScale="30" zoomScaleNormal="91" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="16.8"/>
@@ -45801,7 +45127,7 @@
     <col min="3" max="3" width="47.88671875" style="1" customWidth="1"/>
     <col min="4" max="5" width="48.109375" style="1" customWidth="1"/>
     <col min="6" max="7" width="47.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="47.5546875" style="60" customWidth="1"/>
+    <col min="8" max="8" width="47.5546875" style="46" customWidth="1"/>
     <col min="9" max="11" width="47.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="8.6640625" style="1"/>
@@ -45815,7 +45141,7 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="61"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -45825,12 +45151,12 @@
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
       <c r="K9" s="29"/>
@@ -45840,12 +45166,12 @@
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
@@ -45858,7 +45184,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="62"/>
+      <c r="H11" s="48"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -45873,7 +45199,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="63"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="15" t="s">
         <v>1</v>
       </c>
@@ -45892,7 +45218,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="63"/>
+      <c r="H13" s="49"/>
       <c r="I13" s="15" t="s">
         <v>26</v>
       </c>
@@ -45911,7 +45237,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="63"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="15" t="s">
         <v>5</v>
       </c>
@@ -45930,7 +45256,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="64"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -45947,51 +45273,51 @@
       <c r="G16" s="15"/>
     </row>
     <row r="17" spans="2:11" ht="44.1" customHeight="1">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46" t="s">
+      <c r="E17" s="60"/>
+      <c r="F17" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46" t="s">
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="20.399999999999999" customHeight="1">
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="2:11" ht="120.75" customHeight="1">
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="34" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="H19" s="51" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="34" t="s">
@@ -46000,18 +45326,18 @@
       <c r="J19" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="46"/>
+      <c r="K19" s="60"/>
     </row>
     <row r="20" spans="2:11" s="33" customFormat="1" ht="102" customHeight="1">
       <c r="B20" s="21"/>
       <c r="C20" s="20"/>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="53"/>
+      <c r="E20" s="73"/>
       <c r="F20" s="35"/>
       <c r="G20" s="35"/>
-      <c r="H20" s="58"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="36"/>
       <c r="J20" s="36"/>
       <c r="K20" s="20" t="s">
@@ -46025,7 +45351,7 @@
       <c r="E21" s="37"/>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
-      <c r="H21" s="59"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
       <c r="K21" s="38"/>
@@ -46037,7 +45363,7 @@
       <c r="E22" s="37"/>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
-      <c r="H22" s="59"/>
+      <c r="H22" s="45"/>
       <c r="I22" s="40"/>
       <c r="J22" s="40"/>
       <c r="K22" s="38"/>
@@ -46045,63 +45371,63 @@
     <row r="23" spans="2:11" s="13" customFormat="1" ht="99.9" customHeight="1">
       <c r="B23" s="6"/>
       <c r="C23" s="24"/>
-      <c r="H23" s="66"/>
+      <c r="H23" s="52"/>
     </row>
     <row r="24" spans="2:11" ht="81" customHeight="1">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="47" t="s">
+      <c r="D24" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="47" t="s">
+      <c r="F24" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="64" t="s">
         <v>33</v>
       </c>
       <c r="H24" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="47" t="s">
+      <c r="J24" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="K24" s="50" t="s">
+      <c r="K24" s="70" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="81" customHeight="1">
-      <c r="B25" s="46"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
       <c r="H25" s="68"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="51"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="71"/>
     </row>
     <row r="26" spans="2:11" ht="66.75" customHeight="1">
-      <c r="B26" s="46"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
       <c r="H26" s="69"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="52"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="72"/>
     </row>
     <row r="27" spans="2:11" s="13" customFormat="1" ht="99.9" hidden="1" customHeight="1">
       <c r="B27" s="21" t="s">
@@ -46122,7 +45448,7 @@
       <c r="G27" s="22">
         <v>313.60000000000002</v>
       </c>
-      <c r="H27" s="70" t="s">
+      <c r="H27" s="53" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="23">
@@ -46154,7 +45480,7 @@
       <c r="G28" s="20">
         <v>309.36</v>
       </c>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="53" t="s">
         <v>13</v>
       </c>
       <c r="I28" s="23">
@@ -46186,7 +45512,7 @@
       <c r="G29" s="22">
         <v>298.54000000000002</v>
       </c>
-      <c r="H29" s="70" t="s">
+      <c r="H29" s="53" t="s">
         <v>13</v>
       </c>
       <c r="I29" s="23">
@@ -46206,7 +45532,7 @@
       <c r="E30" s="27"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="71" t="s">
+      <c r="H30" s="54" t="s">
         <v>13</v>
       </c>
       <c r="I30" s="23"/>
@@ -46222,13 +45548,13 @@
       <c r="E31" s="41"/>
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
-      <c r="H31" s="72"/>
+      <c r="H31" s="55"/>
       <c r="I31" s="43"/>
       <c r="J31" s="42"/>
       <c r="K31" s="38"/>
     </row>
     <row r="32" spans="2:11" s="13" customFormat="1" ht="99.9" customHeight="1">
-      <c r="H32" s="66"/>
+      <c r="H32" s="52"/>
     </row>
     <row r="33" spans="2:12" ht="129.9" customHeight="1">
       <c r="B33" s="8"/>
@@ -46237,7 +45563,7 @@
       <c r="E33" s="12"/>
       <c r="F33" s="3"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="73"/>
+      <c r="H33" s="56"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="6"/>
@@ -46250,7 +45576,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="30"/>
       <c r="G34" s="12"/>
-      <c r="H34" s="73"/>
+      <c r="H34" s="56"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="6"/>
@@ -46263,7 +45589,7 @@
       <c r="E35" s="12"/>
       <c r="F35" s="30"/>
       <c r="G35" s="12"/>
-      <c r="H35" s="73"/>
+      <c r="H35" s="56"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="6"/>
@@ -46275,7 +45601,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
-      <c r="H36" s="73"/>
+      <c r="H36" s="56"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="6"/>
@@ -46286,9 +45612,9 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="74"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="57"/>
       <c r="I37" s="6"/>
       <c r="J37" s="7"/>
       <c r="K37" s="6"/>
@@ -46298,7 +45624,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="75"/>
+      <c r="H38" s="58"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -46306,6 +45632,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:E19"/>
+    <mergeCell ref="F17:J18"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="J24:J26"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
@@ -46313,23 +45651,11 @@
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="G24:G26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:E19"/>
-    <mergeCell ref="F17:J18"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="27" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="30" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>